<commit_message>
First step to rebuild
</commit_message>
<xml_diff>
--- a/Rewards1.xlsx
+++ b/Rewards1.xlsx
@@ -418,7 +418,7 @@
   <dimension ref="A1:AJ2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="L2" sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -433,7 +433,9 @@
       <c r="A1" s="1" t="n">
         <v>45058</v>
       </c>
-      <c r="B1" s="1" t="n"/>
+      <c r="B1" s="1" t="n">
+        <v>45058</v>
+      </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -471,6 +473,9 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Adding the ability to switch frames
</commit_message>
<xml_diff>
--- a/Rewards1.xlsx
+++ b/Rewards1.xlsx
@@ -433,9 +433,7 @@
       <c r="A1" s="1" t="n">
         <v>45058</v>
       </c>
-      <c r="B1" s="1" t="n">
-        <v>45058</v>
-      </c>
+      <c r="B1" s="1" t="n"/>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -473,9 +471,6 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
-      </c>
-      <c r="B2" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Yes n No buttons working w the Excel document
</commit_message>
<xml_diff>
--- a/Rewards1.xlsx
+++ b/Rewards1.xlsx
@@ -433,7 +433,9 @@
       <c r="A1" s="1" t="n">
         <v>45058</v>
       </c>
-      <c r="B1" s="1" t="n"/>
+      <c r="B1" s="1" t="n">
+        <v>45058</v>
+      </c>
       <c r="C1" s="1" t="n"/>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -471,6 +473,9 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="n">
         <v>100</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Stuck on the reward amount
</commit_message>
<xml_diff>
--- a/Rewards1.xlsx
+++ b/Rewards1.xlsx
@@ -436,7 +436,9 @@
       <c r="B1" s="1" t="n">
         <v>45058</v>
       </c>
-      <c r="C1" s="1" t="n"/>
+      <c r="C1" s="1" t="n">
+        <v>45058</v>
+      </c>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
       <c r="F1" s="1" t="n"/>
@@ -478,6 +480,9 @@
       <c r="B2" t="n">
         <v>100</v>
       </c>
+      <c r="C2" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>

<commit_message>
No Work Yes No Work
</commit_message>
<xml_diff>
--- a/Rewards1.xlsx
+++ b/Rewards1.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="8880" windowWidth="17280" xWindow="768" yWindow="768"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="12456" windowWidth="23256" xWindow="-108" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
@@ -415,10 +415,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AJ5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L2" sqref="A1:L2"/>
+      <selection activeCell="D5" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4"/>
@@ -431,13 +431,13 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="1" t="n">
-        <v>45058</v>
+        <v>45059</v>
       </c>
       <c r="B1" s="1" t="n">
-        <v>45058</v>
+        <v>45059</v>
       </c>
       <c r="C1" s="1" t="n">
-        <v>45058</v>
+        <v>45059</v>
       </c>
       <c r="D1" s="1" t="n"/>
       <c r="E1" s="1" t="n"/>
@@ -445,9 +445,6 @@
       <c r="G1" s="1" t="n"/>
       <c r="H1" s="1" t="n"/>
       <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
-      <c r="K1" s="1" t="n"/>
-      <c r="L1" s="1" t="n"/>
       <c r="M1" s="1" t="n"/>
       <c r="N1" s="1" t="n"/>
       <c r="O1" s="1" t="n"/>
@@ -475,14 +472,17 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="B2" t="n">
         <v>100</v>
       </c>
       <c r="C2" t="n">
-        <v>0</v>
-      </c>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1" t="n"/>
     </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>

</xml_diff>